<commit_message>
changed the synthesize_text() function in the description.py file
</commit_message>
<xml_diff>
--- a/data/gpt_examples/CProgramming.xlsx
+++ b/data/gpt_examples/CProgramming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Dropbox\twelve-gpt-educational\data\gpt_examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F11B61-0C84-47AA-B69D-5F8FCB657C79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CAF09DF-8127-40D5-A85C-7D0EEF27B8A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,10 +98,10 @@
     <t>assistant</t>
   </si>
   <si>
-    <t>A learner can write the for loop and knows the syntax of the for loop</t>
-  </si>
-  <si>
-    <t>That learner has knowledge of the fgr loop. You should ask the learner complex questions</t>
+    <t>That learner has knowledge of the for loop. You should ask the learner complex questions</t>
+  </si>
+  <si>
+    <t>I can write a for loop</t>
   </si>
 </sst>
 </file>
@@ -1430,7 +1430,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.36328125" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -1438,8 +1438,8 @@
     <col min="1" max="1" width="38.26953125" style="1" customWidth="1"/>
     <col min="2" max="2" width="89.81640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="34.81640625" style="1" customWidth="1"/>
-    <col min="4" max="10" width="8.36328125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.36328125" style="1"/>
+    <col min="4" max="11" width="8.36328125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.36328125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.25" customHeight="1">
@@ -1453,10 +1453,10 @@
     </row>
     <row r="2" spans="1:3" ht="32.25" customHeight="1">
       <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="C2" s="7"/>
     </row>

</xml_diff>